<commit_message>
V2 of the white paper + extra geographica analysis
</commit_message>
<xml_diff>
--- a/data/unknown_LPD.xlsx
+++ b/data/unknown_LPD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP-338\Desktop\ISMI_imputation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP-338\SynologyDrive\git\Abraham\Data_Imputation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,54 +24,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Month</t>
   </si>
   <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>IDP arrivals</t>
-  </si>
-  <si>
-    <t>Returnees</t>
-  </si>
-  <si>
-    <t>Group</t>
+    <t>December-2021</t>
+  </si>
+  <si>
+    <t>January-2022</t>
+  </si>
+  <si>
+    <t>November-2021</t>
+  </si>
+  <si>
+    <t>October-2021</t>
+  </si>
+  <si>
+    <t>September-2021</t>
+  </si>
+  <si>
+    <t>Total # of IDP HH arrivals</t>
+  </si>
+  <si>
+    <t>Sum of # HH LPD</t>
+  </si>
+  <si>
+    <t>Max Cap # HH LPD</t>
+  </si>
+  <si>
+    <t>Percentage_Max_Cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,23 +86,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -385,144 +371,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2">
+        <v>1657</v>
+      </c>
+      <c r="C2">
+        <v>1628</v>
+      </c>
+      <c r="D2">
+        <v>1537</v>
+      </c>
+      <c r="E2">
+        <f>C2/B2</f>
+        <v>0.9824984912492456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>906</v>
+      </c>
+      <c r="C3">
+        <v>899</v>
+      </c>
+      <c r="D3">
+        <v>837</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="0">C3/B3</f>
+        <v>0.99227373068432667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2268</v>
+      </c>
+      <c r="C4">
+        <v>2237</v>
+      </c>
+      <c r="D4">
+        <v>2099</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.98633156966490299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <v>44440</v>
-      </c>
-      <c r="B2" s="5">
-        <v>92.320025653358996</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>44470</v>
-      </c>
-      <c r="B3" s="5">
-        <v>91.943789822815702</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>44501</v>
-      </c>
-      <c r="B4" s="5">
-        <v>92.513823904721406</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>44531</v>
-      </c>
-      <c r="B5" s="5">
-        <v>92.852045670789707</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>44562</v>
-      </c>
-      <c r="B6" s="5">
-        <v>92.282082324455203</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>44440</v>
-      </c>
-      <c r="B7" s="5">
-        <v>72.610784837159599</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>44470</v>
-      </c>
-      <c r="B8" s="5">
-        <v>76.624902114330496</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>44501</v>
-      </c>
-      <c r="B9" s="5">
-        <v>46.820809248554902</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>44531</v>
-      </c>
-      <c r="B10" s="5">
-        <v>30.342516753536898</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>44562</v>
-      </c>
-      <c r="B11" s="5">
-        <v>38.021071919377</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="B5">
+        <v>2240</v>
+      </c>
+      <c r="C5">
+        <v>2183</v>
+      </c>
+      <c r="D5">
+        <v>2059</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.97455357142857146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2397</v>
+      </c>
+      <c r="C6">
+        <v>2336</v>
+      </c>
+      <c r="D6">
+        <v>2211</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.97455152273675427</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>